<commit_message>
Modif des docs rapports et previsions
</commit_message>
<xml_diff>
--- a/bilan prev.xlsx
+++ b/bilan prev.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Documents\GitHub\MasterMind\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="8115" windowHeight="2895"/>
+    <workbookView xWindow="360" yWindow="495" windowWidth="8115" windowHeight="2895"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -94,9 +99,6 @@
   </si>
   <si>
     <t>Version de base qui fonctionne</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>30 min</t>
@@ -127,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +160,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -342,10 +351,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -365,40 +375,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCF0C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCF0C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCF0C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCF0C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -408,6 +395,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -456,7 +446,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,7 +481,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,24 +701,14 @@
     <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -742,7 +722,7 @@
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -766,10 +746,10 @@
         <v>100</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -783,10 +763,10 @@
         <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -800,10 +780,10 @@
         <v>150</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -817,10 +797,10 @@
         <v>1000</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -834,10 +814,10 @@
         <v>100</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -851,10 +831,10 @@
         <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -868,10 +848,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -885,10 +865,10 @@
         <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -902,10 +882,10 @@
         <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -919,10 +899,10 @@
         <v>60</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -936,10 +916,12 @@
         <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="18">
+        <v>0</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -953,10 +935,12 @@
         <v>70</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="18">
+        <v>0</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -970,10 +954,10 @@
         <v>50</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -987,10 +971,12 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="18">
+        <v>1</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1004,10 +990,12 @@
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="18">
+        <v>0</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1021,10 +1009,12 @@
         <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="18">
+        <v>1</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -1038,10 +1028,12 @@
         <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="18">
+        <v>0</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1052,7 +1044,7 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1063,7 +1055,7 @@
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>

</xml_diff>